<commit_message>
Adds 공금대사 SQL and related Excel files
Adds a SQL script for 금액 대사 (fund reconciliation) and associated Excel files.

The SQL script retrieves balance data and calculates various financial aggregates,
including income, expenses, fund balances, and limit allocations.

The Excel files likely serve as templates or reports related to the fund reconciliation process.
</commit_message>
<xml_diff>
--- a/인천보고서_202505(통합).xlsx
+++ b/인천보고서_202505(통합).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\sidogeumgo_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65BE3E9-4C26-4CAA-A1B0-847B43A3B31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366C65F5-4DE3-4E69-AFA5-963E825299C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="93">
   <si>
     <t>품질관리 상세근거</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -530,6 +530,32 @@
 /ui/tom/ich/rpt/xml/ICH030325M01.xml
 crRPTICH030325M01.crf
 tom.ich.rpt.xda.xSelectListICH030325By01.xml</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>금고Cell 시스템 및 업무소개</t>
+  </si>
+  <si>
+    <t>보통예금 부서별 계좌번호 관리</t>
+  </si>
+  <si>
+    <t>2025 보고서 개선</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MMDA, 세입세출외현금 거래구분 추가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>웹취약점 처리</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회계별 잔액 보고서 수정</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>금고운용현황 보고서 수정</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1310,6 +1336,81 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1322,21 +1423,6 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1344,66 +1430,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1722,8 +1748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A38" zoomScale="90" zoomScaleNormal="110" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScale="90" zoomScaleNormal="110" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1740,42 +1766,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="83" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
@@ -1804,44 +1830,46 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="391.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="72" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="86" t="s">
+      <c r="C5" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="90"/>
-      <c r="F5" s="92" t="s">
+      <c r="E5" s="78"/>
+      <c r="F5" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="92" t="s">
+      <c r="G5" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="75"/>
+      <c r="H5" s="63"/>
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="85"/>
+      <c r="A6" s="73"/>
       <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="76"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="64"/>
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="85"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="73"/>
+      <c r="B7" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="C7" s="57">
         <v>2</v>
       </c>
@@ -1857,8 +1885,10 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="85"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="C8" s="57" t="s">
         <v>34</v>
       </c>
@@ -1877,8 +1907,10 @@
       <c r="H8" s="47"/>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="85"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="73"/>
+      <c r="B9" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="C9" s="57">
         <v>7</v>
       </c>
@@ -1898,7 +1930,9 @@
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="223.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="48"/>
-      <c r="B10" s="44"/>
+      <c r="B10" s="44" t="s">
+        <v>88</v>
+      </c>
       <c r="C10" s="57" t="s">
         <v>35</v>
       </c>
@@ -1914,7 +1948,9 @@
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="48"/>
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="C11" s="57">
         <v>8</v>
       </c>
@@ -1930,7 +1966,9 @@
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="48"/>
-      <c r="B12" s="28"/>
+      <c r="B12" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C12" s="57" t="s">
         <v>36</v>
       </c>
@@ -1946,7 +1984,9 @@
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.15">
       <c r="A13" s="48"/>
-      <c r="B13" s="28"/>
+      <c r="B13" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="C13" s="57">
         <v>9</v>
       </c>
@@ -1962,7 +2002,9 @@
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="48"/>
-      <c r="B14" s="28"/>
+      <c r="B14" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C14" s="57" t="s">
         <v>37</v>
       </c>
@@ -1978,7 +2020,9 @@
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="48"/>
-      <c r="B15" s="28"/>
+      <c r="B15" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="C15" s="57">
         <v>12</v>
       </c>
@@ -1994,7 +2038,9 @@
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="48"/>
-      <c r="B16" s="28"/>
+      <c r="B16" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C16" s="57" t="s">
         <v>38</v>
       </c>
@@ -2010,7 +2056,9 @@
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" ht="330" x14ac:dyDescent="0.15">
       <c r="A17" s="48"/>
-      <c r="B17" s="28"/>
+      <c r="B17" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="C17" s="57">
         <v>13</v>
       </c>
@@ -2026,7 +2074,9 @@
     </row>
     <row r="18" spans="1:8" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="48"/>
-      <c r="B18" s="28"/>
+      <c r="B18" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C18" s="57" t="s">
         <v>39</v>
       </c>
@@ -2042,7 +2092,9 @@
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="48"/>
-      <c r="B19" s="28"/>
+      <c r="B19" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="C19" s="57">
         <v>14</v>
       </c>
@@ -2058,7 +2110,9 @@
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" ht="118.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="48"/>
-      <c r="B20" s="28"/>
+      <c r="B20" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C20" s="57" t="s">
         <v>40</v>
       </c>
@@ -2074,7 +2128,9 @@
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" ht="66" x14ac:dyDescent="0.15">
       <c r="A21" s="48"/>
-      <c r="B21" s="28"/>
+      <c r="B21" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="C21" s="57">
         <v>15</v>
       </c>
@@ -2090,7 +2146,9 @@
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="48"/>
-      <c r="B22" s="28"/>
+      <c r="B22" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C22" s="57" t="s">
         <v>41</v>
       </c>
@@ -2106,7 +2164,9 @@
     </row>
     <row r="23" spans="1:8" s="1" customFormat="1" ht="82.5" x14ac:dyDescent="0.15">
       <c r="A23" s="48"/>
-      <c r="B23" s="28"/>
+      <c r="B23" s="28" t="s">
+        <v>89</v>
+      </c>
       <c r="C23" s="57">
         <v>16</v>
       </c>
@@ -2122,7 +2182,9 @@
     </row>
     <row r="24" spans="1:8" s="1" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="48"/>
-      <c r="B24" s="28"/>
+      <c r="B24" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C24" s="57" t="s">
         <v>42</v>
       </c>
@@ -2138,7 +2200,9 @@
     </row>
     <row r="25" spans="1:8" s="1" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="48"/>
-      <c r="B25" s="28"/>
+      <c r="B25" s="28" t="s">
+        <v>89</v>
+      </c>
       <c r="C25" s="57">
         <v>19</v>
       </c>
@@ -2154,7 +2218,9 @@
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="48"/>
-      <c r="B26" s="28"/>
+      <c r="B26" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C26" s="57" t="s">
         <v>43</v>
       </c>
@@ -2170,7 +2236,9 @@
     </row>
     <row r="27" spans="1:8" s="1" customFormat="1" ht="280.5" x14ac:dyDescent="0.15">
       <c r="A27" s="48"/>
-      <c r="B27" s="28"/>
+      <c r="B27" s="28" t="s">
+        <v>89</v>
+      </c>
       <c r="C27" s="57">
         <v>20</v>
       </c>
@@ -2186,7 +2254,9 @@
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1" ht="118.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="48"/>
-      <c r="B28" s="28"/>
+      <c r="B28" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C28" s="57" t="s">
         <v>44</v>
       </c>
@@ -2202,7 +2272,9 @@
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" ht="66" x14ac:dyDescent="0.15">
       <c r="A29" s="48"/>
-      <c r="B29" s="28"/>
+      <c r="B29" s="28" t="s">
+        <v>89</v>
+      </c>
       <c r="C29" s="57">
         <v>21</v>
       </c>
@@ -2218,7 +2290,9 @@
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" ht="192" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="48"/>
-      <c r="B30" s="28"/>
+      <c r="B30" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C30" s="57" t="s">
         <v>45</v>
       </c>
@@ -2234,7 +2308,9 @@
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="48"/>
-      <c r="B31" s="28"/>
+      <c r="B31" s="28" t="s">
+        <v>90</v>
+      </c>
       <c r="C31" s="57">
         <v>22</v>
       </c>
@@ -2250,7 +2326,9 @@
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1" ht="183" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="48"/>
-      <c r="B32" s="28"/>
+      <c r="B32" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C32" s="57" t="s">
         <v>46</v>
       </c>
@@ -2266,7 +2344,9 @@
     </row>
     <row r="33" spans="1:8" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.15">
       <c r="A33" s="48"/>
-      <c r="B33" s="28"/>
+      <c r="B33" s="28" t="s">
+        <v>90</v>
+      </c>
       <c r="C33" s="57">
         <v>23</v>
       </c>
@@ -2282,7 +2362,9 @@
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="48"/>
-      <c r="B34" s="28"/>
+      <c r="B34" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C34" s="57" t="s">
         <v>47</v>
       </c>
@@ -2298,7 +2380,9 @@
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="48"/>
-      <c r="B35" s="28"/>
+      <c r="B35" s="28" t="s">
+        <v>90</v>
+      </c>
       <c r="C35" s="57">
         <v>26</v>
       </c>
@@ -2314,7 +2398,9 @@
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="48"/>
-      <c r="B36" s="28"/>
+      <c r="B36" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C36" s="57" t="s">
         <v>48</v>
       </c>
@@ -2330,7 +2416,9 @@
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.15">
       <c r="A37" s="48"/>
-      <c r="B37" s="28"/>
+      <c r="B37" s="28" t="s">
+        <v>90</v>
+      </c>
       <c r="C37" s="57">
         <v>27</v>
       </c>
@@ -2346,7 +2434,9 @@
     </row>
     <row r="38" spans="1:8" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="48"/>
-      <c r="B38" s="28"/>
+      <c r="B38" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C38" s="57" t="s">
         <v>49</v>
       </c>
@@ -2362,7 +2452,9 @@
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="48"/>
-      <c r="B39" s="28"/>
+      <c r="B39" s="28" t="s">
+        <v>90</v>
+      </c>
       <c r="C39" s="57">
         <v>28</v>
       </c>
@@ -2378,7 +2470,9 @@
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" ht="211.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="48"/>
-      <c r="B40" s="28"/>
+      <c r="B40" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C40" s="57" t="s">
         <v>50</v>
       </c>
@@ -2394,7 +2488,9 @@
     </row>
     <row r="41" spans="1:8" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.15">
       <c r="A41" s="48"/>
-      <c r="B41" s="28"/>
+      <c r="B41" s="28" t="s">
+        <v>91</v>
+      </c>
       <c r="C41" s="57">
         <v>29</v>
       </c>
@@ -2410,7 +2506,9 @@
     </row>
     <row r="42" spans="1:8" s="1" customFormat="1" ht="195.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="48"/>
-      <c r="B42" s="28"/>
+      <c r="B42" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="C42" s="57" t="s">
         <v>51</v>
       </c>
@@ -2426,7 +2524,9 @@
     </row>
     <row r="43" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A43" s="48"/>
-      <c r="B43" s="28"/>
+      <c r="B43" s="28" t="s">
+        <v>92</v>
+      </c>
       <c r="C43" s="57" t="s">
         <v>51</v>
       </c>
@@ -2451,19 +2551,19 @@
       <c r="H44" s="54"/>
     </row>
     <row r="45" spans="1:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="77" t="s">
+      <c r="A45" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="94" t="s">
+      <c r="B45" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="69" t="s">
+      <c r="C45" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="93" t="s">
+      <c r="D45" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="94" t="s">
+      <c r="E45" s="85" t="s">
         <v>25</v>
       </c>
       <c r="F45" s="24" t="s">
@@ -2475,21 +2575,21 @@
       <c r="H45" s="25"/>
     </row>
     <row r="46" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="77"/>
-      <c r="B46" s="67"/>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70"/>
-      <c r="E46" s="67"/>
+      <c r="A46" s="65"/>
+      <c r="B46" s="86"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="86"/>
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
       <c r="H46" s="25"/>
     </row>
     <row r="47" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="77"/>
-      <c r="B47" s="67"/>
-      <c r="C47" s="70"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="67"/>
+      <c r="A47" s="65"/>
+      <c r="B47" s="86"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="82"/>
+      <c r="E47" s="86"/>
       <c r="F47" s="13" t="s">
         <v>15</v>
       </c>
@@ -2499,17 +2599,17 @@
       <c r="H47" s="15"/>
     </row>
     <row r="48" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="77"/>
-      <c r="B48" s="68"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="68"/>
+      <c r="A48" s="65"/>
+      <c r="B48" s="87"/>
+      <c r="C48" s="83"/>
+      <c r="D48" s="83"/>
+      <c r="E48" s="87"/>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="15"/>
     </row>
     <row r="49" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="77"/>
+      <c r="A49" s="65"/>
       <c r="B49" s="11"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
@@ -2523,7 +2623,7 @@
       <c r="H49" s="15"/>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="77"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="28"/>
       <c r="C50" s="49"/>
       <c r="D50" s="49"/>
@@ -2533,19 +2633,19 @@
       <c r="H50" s="33"/>
     </row>
     <row r="51" spans="1:8" s="40" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="63" t="s">
+      <c r="A51" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B51" s="66" t="s">
+      <c r="B51" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="C51" s="69" t="s">
+      <c r="C51" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="69" t="s">
+      <c r="D51" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E51" s="72" t="s">
+      <c r="E51" s="92" t="s">
         <v>27</v>
       </c>
       <c r="F51" s="38" t="s">
@@ -2557,21 +2657,21 @@
       <c r="H51" s="39"/>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="64"/>
-      <c r="B52" s="67"/>
-      <c r="C52" s="70"/>
-      <c r="D52" s="70"/>
-      <c r="E52" s="73"/>
+      <c r="A52" s="89"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="93"/>
       <c r="F52" s="24"/>
       <c r="G52" s="24"/>
       <c r="H52" s="25"/>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="64"/>
-      <c r="B53" s="67"/>
-      <c r="C53" s="70"/>
-      <c r="D53" s="70"/>
-      <c r="E53" s="73"/>
+      <c r="A53" s="89"/>
+      <c r="B53" s="86"/>
+      <c r="C53" s="82"/>
+      <c r="D53" s="82"/>
+      <c r="E53" s="93"/>
       <c r="F53" s="13" t="s">
         <v>15</v>
       </c>
@@ -2581,17 +2681,17 @@
       <c r="H53" s="15"/>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="64"/>
-      <c r="B54" s="68"/>
-      <c r="C54" s="71"/>
-      <c r="D54" s="71"/>
-      <c r="E54" s="74"/>
+      <c r="A54" s="89"/>
+      <c r="B54" s="87"/>
+      <c r="C54" s="83"/>
+      <c r="D54" s="83"/>
+      <c r="E54" s="94"/>
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
       <c r="H54" s="15"/>
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="64"/>
+      <c r="A55" s="89"/>
       <c r="B55" s="11" t="s">
         <v>29</v>
       </c>
@@ -2613,7 +2713,7 @@
       <c r="H55" s="15"/>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="64"/>
+      <c r="A56" s="89"/>
       <c r="B56" s="11" t="s">
         <v>73</v>
       </c>
@@ -2631,7 +2731,7 @@
       <c r="H56" s="15"/>
     </row>
     <row r="57" spans="1:8" s="27" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="65"/>
+      <c r="A57" s="90"/>
       <c r="B57" s="17"/>
       <c r="C57" s="41"/>
       <c r="D57" s="41"/>
@@ -2808,6 +2908,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="D51:D54"/>
+    <mergeCell ref="E51:E54"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="A45:A50"/>
     <mergeCell ref="A1:H1"/>
@@ -2824,11 +2929,6 @@
     <mergeCell ref="D45:D48"/>
     <mergeCell ref="E45:E48"/>
     <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="E51:E54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.3" right="0" top="0.3" bottom="0.11811023622047245" header="0.22" footer="0.19685039370078741"/>

</xml_diff>